<commit_message>
modified template, added conditional formatting
</commit_message>
<xml_diff>
--- a/BTT_Template.xlsx
+++ b/BTT_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamueller\PycharmProjects\btt_concat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E5A2B5-8A87-4E86-AE1C-0EC58034CA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705094D6-4AAA-485E-9202-2A8B7D7281DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-67320" yWindow="4770" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="8" r:id="rId1"/>
@@ -2646,7 +2646,106 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFA7A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2873,8 +2972,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Teilprojekte"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Kürzel"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Anfangszeile" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Endzeile" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Anfangszeile" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Endzeile" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2921,7 +3020,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="BTT" displayName="BTT" ref="A2:AT530" totalsRowShown="0" headerRowDxfId="24" dataCellStyle="Standard">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="BTT" displayName="BTT" ref="A2:AT530" totalsRowShown="0" headerRowDxfId="38" dataCellStyle="Standard">
   <autoFilter ref="A2:AT530" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="46">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Lfd Nr._x000a_(automatisch)" dataCellStyle="Standard"/>
@@ -2991,7 +3090,7 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Hauptprozess"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="ARIS-ID"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Verantwortliches TP"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="verwendet in BTT" dataDxfId="23">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="verwendet in BTT" dataDxfId="37">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(Hauptprozesse[[#This Row],[Hauptprozess]],BTT[Hauptprozess
 (Pflichtauswahl)],1,FALSE)),"nein","ja")</calculatedColumnFormula>
     </tableColumn>
@@ -3010,10 +3109,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Subprozess"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ARIS-ID"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Zugeordneter Hauptprozess"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="TP aus Hauptprozess" dataDxfId="22">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="TP aus Hauptprozess" dataDxfId="36">
       <calculatedColumnFormula>VLOOKUP(BPML[[#This Row],[Zugeordneter Hauptprozess]],Hauptprozesse[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="verwendet in BTT" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="verwendet in BTT" dataDxfId="35">
       <calculatedColumnFormula>IF(ISERROR(VLOOKUP(BPML[[#This Row],[Subprozess]],BTT[Subprozess
 (optionale Auswahl)],1,FALSE)),"nein","ja")</calculatedColumnFormula>
     </tableColumn>
@@ -3056,9 +3155,9 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Transaktionen"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Langtext"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Modul"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Anzahl Nutzungen (2022+2023)" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Anzahl Nutzungen (2022+2023)" dataDxfId="34"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Tasktyp"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="verwendet in BTT" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="verwendet in BTT" dataDxfId="33"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Bemerkungen"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3071,7 +3170,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Formularbezeichnung"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Formularname (technisch)"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="verwendet in BTT" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="verwendet in BTT" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3088,8 +3187,8 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Namespace"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="SenderServiceInterface"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Receiver"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Wo ist Mandant 100" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="erzeugter Name" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Wo ist Mandant 100" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="erzeugter Name" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3104,7 +3203,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Schnittstelle"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Beschreibung System"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="verwendet in BTT" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="verwendet in BTT" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3119,7 +3218,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Module"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Bezeichnung"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Modul in Transaktionen" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Modul in Transaktionen" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3799,76 +3898,6 @@
     <mergeCell ref="E1:Z1"/>
     <mergeCell ref="AK1:AT1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:B530">
-    <cfRule type="expression" dxfId="13" priority="24">
-      <formula>ISBLANK(B3)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D530 H3:I530 O3:O530 T3:T530 X3:X530 Z3:Z530 AD3:AD530 AI3:AJ530">
-    <cfRule type="expression" dxfId="12" priority="26">
-      <formula>ISBLANK(D3)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="U3:V530">
-    <cfRule type="expression" dxfId="11" priority="19">
-      <formula>AND(ISBLANK(U3),T3="SAP-Formular")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="W3:W530">
-    <cfRule type="expression" dxfId="10" priority="18">
-      <formula>AND(ISBLANK(W3),OR(T3="Mail",T3="XML",T3="weiterer"))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA3:AA530">
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>AND(ISBLANK(AA3),NOT(ISBLANK(I3)),LEFT(I3,1)="Z")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB530">
-    <cfRule type="expression" dxfId="8" priority="14">
-      <formula>AND(ISBLANK(AB3),NOT(ISBLANK(I3)),LEFT(I3,1)&lt;&gt;"Z")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE273 AE292:AE530">
-    <cfRule type="expression" dxfId="7" priority="12">
-      <formula>AND(ISBLANK(AE3),AB3="ja")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE274:AE291">
-    <cfRule type="expression" dxfId="6" priority="4">
-      <formula>ISBLANK(AE274)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF3:AF307 AF310:AF321 AF326 AF331:AF333 AF335:AF530">
-    <cfRule type="expression" dxfId="5" priority="11">
-      <formula>AND(ISBLANK(AF3),AD3="Fiori")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF308:AF309">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>ISBLANK(AF308)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF322:AF325">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>ISBLANK(AF322)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF327:AF330">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>ISBLANK(AF327)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG3:AG530">
-    <cfRule type="expression" dxfId="1" priority="9">
-      <formula>AND(ISBLANK(AG3),NOT(ISBLANK(M3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH530">
-    <cfRule type="expression" dxfId="0" priority="8">
-      <formula>AND(ISBLANK(AH3),NOT(ISBLANK(R3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B530" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>Hauptprozess</formula1>
@@ -6528,7 +6557,7 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:G4278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -19512,8 +19541,8 @@
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19575,6 +19604,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DokumenteTeilen_x0020__x002d__x0020_Berechtigungen xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </DokumenteTeilen_x0020__x002d__x0020_Berechtigungen>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="079a195e-b63e-432e-9525-85ffc651ce0e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005C17858E2359B24DBC2C956CBC58571A" ma:contentTypeVersion="23" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2500c3fdc20045965f25a0a7c11fd3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3d735070-d042-4b9b-adb1-ed729648994d" xmlns:ns3="079a195e-b63e-432e-9525-85ffc651ce0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04b8bdc2aec7392572213476c7d3400a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19865,21 +19909,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DokumenteTeilen_x0020__x002d__x0020_Berechtigungen xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </DokumenteTeilen_x0020__x002d__x0020_Berechtigungen>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="079a195e-b63e-432e-9525-85ffc651ce0e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6D06BF-D986-40C6-9747-40ACA7005104}">
   <ds:schemaRefs>
@@ -19889,6 +19918,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8939E25B-C81C-45B1-8008-CF142999BF4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3d735070-d042-4b9b-adb1-ed729648994d"/>
+    <ds:schemaRef ds:uri="079a195e-b63e-432e-9525-85ffc651ce0e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3B6455-98BE-4DD6-ACF3-BBC2A457E6E8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19906,15 +19946,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8939E25B-C81C-45B1-8008-CF142999BF4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3d735070-d042-4b9b-adb1-ed729648994d"/>
-    <ds:schemaRef ds:uri="079a195e-b63e-432e-9525-85ffc651ce0e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final push for this version
</commit_message>
<xml_diff>
--- a/BTT_Template.xlsx
+++ b/BTT_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamueller\PycharmProjects\btt_concat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55419EC-3A67-4408-AE07-4B04E0F1697F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD63D37-01BB-4760-8D34-1F4E87D4FD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67320" yWindow="4770" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5595" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="8" r:id="rId1"/>
@@ -1957,8 +1957,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Schnittstellen_technisch" displayName="Schnittstellen_technisch" ref="A1:F141" totalsRowShown="0">
-  <autoFilter ref="A1:F141" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Schnittstellen_technisch" displayName="Schnittstellen_technisch" ref="A1:F2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F176">
     <sortCondition descending="1" ref="E1:E176"/>
   </sortState>
@@ -2320,7 +2320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E342597-281F-452D-8331-F7EAFBB9CD2B}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
@@ -2727,8 +2727,8 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15709,19 +15709,19 @@
   <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="21" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -15772,7 +15772,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="A2" sqref="A2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15825,21 +15825,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DokumenteTeilen_x0020__x002d__x0020_Berechtigungen xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </DokumenteTeilen_x0020__x002d__x0020_Berechtigungen>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="079a195e-b63e-432e-9525-85ffc651ce0e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005C17858E2359B24DBC2C956CBC58571A" ma:contentTypeVersion="23" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="a2500c3fdc20045965f25a0a7c11fd3f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3d735070-d042-4b9b-adb1-ed729648994d" xmlns:ns3="079a195e-b63e-432e-9525-85ffc651ce0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04b8bdc2aec7392572213476c7d3400a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16130,6 +16115,21 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DokumenteTeilen_x0020__x002d__x0020_Berechtigungen xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </DokumenteTeilen_x0020__x002d__x0020_Berechtigungen>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="079a195e-b63e-432e-9525-85ffc651ce0e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -16140,17 +16140,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8939E25B-C81C-45B1-8008-CF142999BF4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3d735070-d042-4b9b-adb1-ed729648994d"/>
-    <ds:schemaRef ds:uri="079a195e-b63e-432e-9525-85ffc651ce0e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE3B6455-98BE-4DD6-ACF3-BBC2A457E6E8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16170,6 +16159,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8939E25B-C81C-45B1-8008-CF142999BF4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3d735070-d042-4b9b-adb1-ed729648994d"/>
+    <ds:schemaRef ds:uri="079a195e-b63e-432e-9525-85ffc651ce0e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6D06BF-D986-40C6-9747-40ACA7005104}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
new branch for new BWB requirements
</commit_message>
<xml_diff>
--- a/BTT_Template.xlsx
+++ b/BTT_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pamueller\PycharmProjects\btt_concat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD63D37-01BB-4760-8D34-1F4E87D4FD90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B8AC7A-7D54-4CBD-910B-8C05DFD25E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5595" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5595" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="8" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="Schnittstellen" sheetId="5" r:id="rId6"/>
     <sheet name="Datengrundlage adesso" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="aktives_Teilprojekt">Übersicht!$A$1</definedName>
+  </definedNames>
   <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -533,7 +536,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>Qualitätssicherung</t>
   </si>
@@ -1415,12 +1418,6 @@
     <t>Interfaces</t>
   </si>
   <si>
-    <t>Business Transformation Tracker</t>
-  </si>
-  <si>
-    <t>Finanzen</t>
-  </si>
-  <si>
     <t>Endzeile</t>
   </si>
   <si>
@@ -1431,6 +1428,9 @@
   </si>
   <si>
     <t>Teilprojekte</t>
+  </si>
+  <si>
+    <t>Master</t>
   </si>
 </sst>
 </file>
@@ -2321,7 +2321,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,20 +2333,20 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B1" s="14"/>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2418,11 +2418,11 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:AT351"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="AN3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,8 +2473,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
-        <v>79</v>
+      <c r="A1" s="17" t="str">
+        <f>"Business Transformation Tracker: "&amp;aktives_Teilprojekt</f>
+        <v>Business Transformation Tracker: Master</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -15709,7 +15710,7 @@
   <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -16116,6 +16117,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <DokumenteTeilen_x0020__x002d__x0020_Berechtigungen xmlns="3d735070-d042-4b9b-adb1-ed729648994d">
@@ -16128,15 +16138,6 @@
     <TaxCatchAll xmlns="079a195e-b63e-432e-9525-85ffc651ce0e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16160,6 +16161,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6D06BF-D986-40C6-9747-40ACA7005104}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8939E25B-C81C-45B1-8008-CF142999BF4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -16168,12 +16177,4 @@
     <ds:schemaRef ds:uri="079a195e-b63e-432e-9525-85ffc651ce0e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6D06BF-D986-40C6-9747-40ACA7005104}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>